<commit_message>
lab 2 CMake + 2_5_1 update
</commit_message>
<xml_diff>
--- a/2_semester/labs/lab_2_5_1/2_5_1.xlsx
+++ b/2_semester/labs/lab_2_5_1/2_5_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mipt_dgap\2_semester\labs\lab_2_5_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\mipt_dgap\2_semester\labs\lab_2_5_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A0F032-1E2A-4ADB-AB7C-0F93DB02194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C33AA3-44CB-4696-85D8-D6989BAED4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{438C22A8-7B93-426B-B172-54550A05B405}"/>
+    <workbookView minimized="1" xWindow="1755" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{438C22A8-7B93-426B-B172-54550A05B405}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -616,24 +616,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA98A08D-1FA0-4A65-B8DB-055746EF8A50}">
   <dimension ref="B1:Z68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="8.88671875" style="1"/>
-    <col min="13" max="13" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.33203125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="1"/>
-    <col min="16" max="16" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="1"/>
-    <col min="18" max="18" width="10.33203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="12" width="8.85546875" style="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="1"/>
+    <col min="16" max="16" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="10.28515625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -690,12 +690,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>0.5</v>
+        <v>129</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -746,7 +746,7 @@
       </c>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -785,7 +785,7 @@
       </c>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -824,7 +824,7 @@
       </c>
       <c r="Z5" s="10"/>
     </row>
-    <row r="6" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -832,13 +832,13 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1">
         <f>C3*C4*C5</f>
-        <v>0.98066500000000001</v>
+        <v>253.01157000000001</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>6</v>
@@ -896,7 +896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
@@ -968,7 +968,7 @@
         <v>224.3</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F9" s="6"/>
       <c r="G9" s="2">
         <v>2</v>
@@ -1028,7 +1028,7 @@
         <v>224.3</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F10" s="6" t="s">
         <v>1</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>224.33333333333334</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F11" s="6">
         <v>0.2</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>224.16666666666666</v>
       </c>
     </row>
-    <row r="12" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="8"/>
       <c r="G12" s="9">
         <v>5</v>
@@ -1220,7 +1220,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O13" s="1">
         <f>45+273</f>
         <v>318</v>
@@ -1240,7 +1240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F15" s="6">
         <v>28</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="F16" s="6"/>
       <c r="G16" s="2">
         <v>2</v>
@@ -1428,7 +1428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F17" s="6" t="s">
         <v>1</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>439.33792</v>
       </c>
     </row>
-    <row r="18" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F18" s="6">
         <v>0.2</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="8"/>
       <c r="G19" s="9">
         <v>5</v>
@@ -1570,7 +1570,7 @@
         <v>295</v>
       </c>
       <c r="P19" s="15">
-        <f>-O19*N19</f>
+        <f t="shared" ref="P19:P27" si="5">-O19*N19</f>
         <v>8.678850833334209E-3</v>
       </c>
       <c r="Q19" s="1">
@@ -1602,7 +1602,7 @@
         <v>0.131801376</v>
       </c>
     </row>
-    <row r="20" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N20" s="13">
         <v>2.4841304445577199E-18</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>301</v>
       </c>
       <c r="P20" s="15">
-        <f>-O20*N20</f>
+        <f t="shared" si="5"/>
         <v>-7.4772326381187367E-16</v>
       </c>
       <c r="Q20" s="1">
@@ -1623,7 +1623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F21" s="3" t="s">
         <v>6</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>305</v>
       </c>
       <c r="P21" s="15">
-        <f>-O21*N21</f>
+        <f t="shared" si="5"/>
         <v>5.3838600000000306E-2</v>
       </c>
       <c r="Q21" s="1">
@@ -1684,7 +1684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F22" s="6">
         <v>32</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" ref="I22:I26" si="5">(J22-K22)^2</f>
+        <f t="shared" ref="I22:I26" si="6">(J22-K22)^2</f>
         <v>0</v>
       </c>
       <c r="J22" s="2">
@@ -1720,7 +1720,7 @@
         <v>308</v>
       </c>
       <c r="P22" s="15">
-        <f>-O22*N22</f>
+        <f t="shared" si="5"/>
         <v>4.7118948800002156E-2</v>
       </c>
       <c r="Q22" s="1">
@@ -1753,7 +1753,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F23" s="6"/>
       <c r="G23" s="2">
         <v>2</v>
@@ -1762,7 +1762,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J23" s="2">
@@ -1782,7 +1782,7 @@
         <v>313</v>
       </c>
       <c r="P23" s="15">
-        <f>-O23*N23</f>
+        <f t="shared" si="5"/>
         <v>5.8934081399997493E-2</v>
       </c>
       <c r="Q23" s="1">
@@ -1812,7 +1812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F24" s="6" t="s">
         <v>1</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J24" s="2">
@@ -1845,7 +1845,7 @@
         <v>318</v>
       </c>
       <c r="P24" s="15">
-        <f>-O24*N24</f>
+        <f t="shared" si="5"/>
         <v>0.10103985720000128</v>
       </c>
       <c r="Q24" s="1">
@@ -1878,7 +1878,7 @@
         <v>439.33792</v>
       </c>
     </row>
-    <row r="25" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F25" s="6">
         <v>0.2</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>25</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J25" s="2">
@@ -1909,7 +1909,7 @@
         <v>323</v>
       </c>
       <c r="P25" s="15">
-        <f>-O25*N25</f>
+        <f t="shared" si="5"/>
         <v>5.7015830799997419E-2</v>
       </c>
       <c r="Q25" s="1">
@@ -1941,7 +1941,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F26" s="8"/>
       <c r="G26" s="9">
         <v>5</v>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J26" s="9">
@@ -1972,7 +1972,7 @@
         <v>328</v>
       </c>
       <c r="P26" s="15">
-        <f>-O26*N26</f>
+        <f t="shared" si="5"/>
         <v>6.7548238000006894E-2</v>
       </c>
       <c r="Q26" s="1">
@@ -2003,7 +2003,7 @@
         <v>0.131801376</v>
       </c>
     </row>
-    <row r="27" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N27" s="14">
         <v>-2.05939750000021E-4</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>332</v>
       </c>
       <c r="P27" s="15">
-        <f>-O27*N27</f>
+        <f t="shared" si="5"/>
         <v>6.837199700000697E-2</v>
       </c>
       <c r="Q27" s="1">
@@ -2024,7 +2024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F28" s="3" t="s">
         <v>6</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F29" s="6">
         <v>35</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" ref="I29:I33" si="6">(J29-K29)^2</f>
+        <f t="shared" ref="I29:I33" si="7">(J29-K29)^2</f>
         <v>0.81000000000001027</v>
       </c>
       <c r="J29" s="2">
@@ -2131,7 +2131,7 @@
         <v>223.1</v>
       </c>
     </row>
-    <row r="30" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F30" s="6"/>
       <c r="G30" s="2">
         <v>2</v>
@@ -2140,7 +2140,7 @@
         <v>24</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.999999999998864E-3</v>
       </c>
       <c r="J30" s="2">
@@ -2187,7 +2187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F31" s="6" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>0.54772255750516619</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.999999999998864E-3</v>
       </c>
       <c r="J31" s="2">
@@ -2217,7 +2217,7 @@
         <v>301</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" ref="P31:P38" si="7">P9+P20</f>
+        <f t="shared" ref="P31:P38" si="8">P9+P20</f>
         <v>8.0316463499999241E-2</v>
       </c>
       <c r="Q31" s="1">
@@ -2250,7 +2250,7 @@
         <v>437.572723</v>
       </c>
     </row>
-    <row r="32" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F32" s="6">
         <v>0.2</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>25</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.35999999999999316</v>
       </c>
       <c r="J32" s="2">
@@ -2278,7 +2278,7 @@
         <v>305</v>
       </c>
       <c r="P32" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.13415506350000028</v>
       </c>
       <c r="Q32" s="1">
@@ -2310,7 +2310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F33" s="8"/>
       <c r="G33" s="9">
         <v>5</v>
@@ -2320,7 +2320,7 @@
         <v>3.2227940511348228E-4</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.999999999998864E-3</v>
       </c>
       <c r="J33" s="9">
@@ -2338,7 +2338,7 @@
         <v>308</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.12690585320000214</v>
       </c>
       <c r="Q33" s="1">
@@ -2369,12 +2369,12 @@
         <v>0.13127181689999998</v>
       </c>
     </row>
-    <row r="34" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O34" s="1">
         <v>313</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.1379560670999975</v>
       </c>
       <c r="Q34" s="1">
@@ -2387,7 +2387,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F35" s="3" t="s">
         <v>6</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>318</v>
       </c>
       <c r="P35" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.17912040450000127</v>
       </c>
       <c r="Q35" s="1">
@@ -2445,7 +2445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F36" s="6">
         <v>40</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>0.8</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" ref="I36:I40" si="8">(J36-K36)^2</f>
+        <f t="shared" ref="I36:I40" si="9">(J36-K36)^2</f>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J36" s="2">
@@ -2478,7 +2478,7 @@
         <v>323</v>
       </c>
       <c r="P36" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.13350770079999741</v>
       </c>
       <c r="Q36" s="1">
@@ -2511,7 +2511,7 @@
         <v>221.8</v>
       </c>
     </row>
-    <row r="37" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F37" s="6"/>
       <c r="G37" s="2">
         <v>2</v>
@@ -2520,7 +2520,7 @@
         <v>24</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J37" s="2">
@@ -2537,7 +2537,7 @@
         <v>328</v>
       </c>
       <c r="P37" s="1">
-        <f t="shared" si="7"/>
+        <f>P15+P26</f>
         <v>0.14315750950000689</v>
       </c>
       <c r="Q37" s="1">
@@ -2567,7 +2567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F38" s="6" t="s">
         <v>1</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0.44721359549995793</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.64000000000001822</v>
       </c>
       <c r="J38" s="2">
@@ -2597,7 +2597,7 @@
         <v>332</v>
       </c>
       <c r="P38" s="1">
-        <f t="shared" si="7"/>
+        <f>P16+P27</f>
         <v>0.14315750990000697</v>
       </c>
       <c r="Q38" s="1">
@@ -2630,7 +2630,7 @@
         <v>435.02299400000004</v>
       </c>
     </row>
-    <row r="39" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F39" s="6">
         <v>0.2</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J39" s="2">
@@ -2674,7 +2674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F40" s="8"/>
       <c r="G40" s="9">
         <v>5</v>
@@ -2684,7 +2684,7 @@
         <v>2.6314003237857972E-4</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J40" s="9">
@@ -2717,8 +2717,8 @@
         <v>0.1305068982</v>
       </c>
     </row>
-    <row r="41" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F42" s="3" t="s">
         <v>6</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F43" s="6">
         <v>45</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0.80000000000000016</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" ref="I43:I47" si="9">(J43-K43)^2</f>
+        <f t="shared" ref="I43:I47" si="10">(J43-K43)^2</f>
         <v>0.64000000000001822</v>
       </c>
       <c r="J43" s="2">
@@ -2810,7 +2810,7 @@
         <v>220.2</v>
       </c>
     </row>
-    <row r="44" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F44" s="6"/>
       <c r="G44" s="2">
         <v>2</v>
@@ -2819,7 +2819,7 @@
         <v>24</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J44" s="2">
@@ -2850,7 +2850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F45" s="6" t="s">
         <v>1</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>0.44721359549995798</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J45" s="2">
@@ -2897,7 +2897,7 @@
         <v>431.88486599999999</v>
       </c>
     </row>
-    <row r="46" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F46" s="6">
         <v>0.2</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>25</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J46" s="2">
@@ -2941,7 +2941,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F47" s="8"/>
       <c r="G47" s="9">
         <v>5</v>
@@ -2951,7 +2951,7 @@
         <v>2.6314003237857978E-4</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.9999999999995456E-2</v>
       </c>
       <c r="J47" s="9">
@@ -2984,8 +2984,8 @@
         <v>0.12956545979999998</v>
       </c>
     </row>
-    <row r="48" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F49" s="3" t="s">
         <v>6</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F50" s="6">
         <v>50</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" ref="I50:I54" si="10">(J50-K50)^2</f>
+        <f t="shared" ref="I50:I54" si="11">(J50-K50)^2</f>
         <v>0.25</v>
       </c>
       <c r="J50" s="2">
@@ -3077,7 +3077,7 @@
         <v>217.5</v>
       </c>
     </row>
-    <row r="51" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F51" s="6"/>
       <c r="G51" s="2">
         <v>2</v>
@@ -3086,7 +3086,7 @@
         <v>24</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="J51" s="2">
@@ -3117,7 +3117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F52" s="6" t="s">
         <v>1</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>0.5</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J52" s="2">
@@ -3164,7 +3164,7 @@
         <v>426.58927499999999</v>
       </c>
     </row>
-    <row r="53" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F53" s="6">
         <v>0.2</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>25</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="J53" s="2">
@@ -3208,7 +3208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F54" s="8"/>
       <c r="G54" s="9">
         <v>5</v>
@@ -3218,7 +3218,7 @@
         <v>2.9419949999999999E-4</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="J54" s="9">
@@ -3251,8 +3251,8 @@
         <v>0.1279767825</v>
       </c>
     </row>
-    <row r="55" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F56" s="3" t="s">
         <v>6</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F57" s="6">
         <v>55</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" ref="I57:I61" si="11">(J57-K57)^2</f>
+        <f t="shared" ref="I57:I61" si="12">(J57-K57)^2</f>
         <v>0</v>
       </c>
       <c r="J57" s="2">
@@ -3344,7 +3344,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F58" s="6"/>
       <c r="G58" s="2">
         <v>2</v>
@@ -3353,7 +3353,7 @@
         <v>24</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J58" s="2">
@@ -3384,7 +3384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F59" s="6" t="s">
         <v>1</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>0</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J59" s="2">
@@ -3431,7 +3431,7 @@
         <v>423.64728000000002</v>
       </c>
     </row>
-    <row r="60" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F60" s="6">
         <v>0.2</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>25</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J60" s="2">
@@ -3475,7 +3475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F61" s="8"/>
       <c r="G61" s="9">
         <v>5</v>
@@ -3485,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J61" s="9">
@@ -3518,8 +3518,8 @@
         <v>0.127094184</v>
       </c>
     </row>
-    <row r="62" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F63" s="3" t="s">
         <v>6</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F64" s="6">
         <v>59</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>1.2</v>
       </c>
       <c r="I64" s="2">
-        <f t="shared" ref="I64:I68" si="12">(J64-K64)^2</f>
+        <f t="shared" ref="I64:I68" si="13">(J64-K64)^2</f>
         <v>0.16000000000000456</v>
       </c>
       <c r="J64" s="2">
@@ -3611,7 +3611,7 @@
         <v>214.6</v>
       </c>
     </row>
-    <row r="65" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F65" s="6"/>
       <c r="G65" s="2">
         <v>2</v>
@@ -3620,7 +3620,7 @@
         <v>24</v>
       </c>
       <c r="I65" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.16000000000000456</v>
       </c>
       <c r="J65" s="2">
@@ -3651,7 +3651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F66" s="6" t="s">
         <v>1</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>0.54772255750516607</v>
       </c>
       <c r="I66" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.16000000000000456</v>
       </c>
       <c r="J66" s="2">
@@ -3698,7 +3698,7 @@
         <v>420.90141799999998</v>
       </c>
     </row>
-    <row r="67" spans="6:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F67" s="6">
         <v>0.2</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>25</v>
       </c>
       <c r="I67" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.35999999999999316</v>
       </c>
       <c r="J67" s="2">
@@ -3742,7 +3742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="6:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F68" s="8"/>
       <c r="G68" s="9">
         <v>5</v>
@@ -3752,7 +3752,7 @@
         <v>3.2227940511348223E-4</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.35999999999999316</v>
       </c>
       <c r="J68" s="9">

</xml_diff>